<commit_message>
updated our examples updated allfunctions
</commit_message>
<xml_diff>
--- a/templates/EmpaticaOnly/0.RawData/ParticipantData.xlsx
+++ b/templates/EmpaticaOnly/0.RawData/ParticipantData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EXP_Lab\SVN\templates\EmpaticaOnly\0.RawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\EXP_Lab\ExperienceLabPipelineGit\templates\EmpaticaOnly\0.RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47644EA7-51A2-4A7F-9EC6-2B3A8F5E0D80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32231ED4-5E1D-408E-9398-5FE18F74E8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10125" yWindow="690" windowWidth="16590" windowHeight="20310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39390" yWindow="2805" windowWidth="23460" windowHeight="17490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="14">
   <si>
     <t>Participant</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Out</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
+    <t>Europe/Amsterdam</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,9 +420,10 @@
     <col min="2" max="3" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,8 +442,11 @@
       <c r="F1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -456,8 +466,11 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -477,8 +490,11 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -498,8 +514,11 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -519,8 +538,11 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>12</v>
       </c>
@@ -540,8 +562,11 @@
       <c r="F6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>13</v>
       </c>
@@ -561,8 +586,11 @@
       <c r="F7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>14</v>
       </c>
@@ -582,8 +610,11 @@
       <c r="F8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16</v>
       </c>
@@ -603,8 +634,11 @@
       <c r="F9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17</v>
       </c>
@@ -624,8 +658,11 @@
       <c r="F10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>18</v>
       </c>
@@ -645,8 +682,11 @@
       <c r="F11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>22</v>
       </c>
@@ -666,8 +706,11 @@
       <c r="F12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>23</v>
       </c>
@@ -686,6 +729,9 @@
       </c>
       <c r="F13" t="s">
         <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>